<commit_message>
Ok consulta incidentes desde soporte
</commit_message>
<xml_diff>
--- a/grexco/scripts/crear_reportes.xlsx
+++ b/grexco/scripts/crear_reportes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arju\Desktop\Grexco\Proyectos\Web\grexco\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C976A567-83FD-447C-821F-4E1457CF1E12}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20728CC-E4D6-4979-B70E-CDA9DF0F0A04}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="8520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Reporte</t>
   </si>
@@ -28,10 +28,109 @@
     <t>id App</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
+    <t>GarProVen</t>
+  </si>
+  <si>
+    <t>GrexActFij</t>
+  </si>
+  <si>
+    <t>GrexMsgs</t>
+  </si>
+  <si>
+    <t>grexrepo</t>
+  </si>
+  <si>
+    <t>HisManAct</t>
+  </si>
+  <si>
+    <t>HVActivo</t>
+  </si>
+  <si>
+    <t>InvActDep</t>
+  </si>
+  <si>
+    <t>InvActPer.sql</t>
+  </si>
+  <si>
+    <t>InvCom1</t>
+  </si>
+  <si>
+    <t>InvComp</t>
+  </si>
+  <si>
+    <t>InveDepTpl</t>
+  </si>
+  <si>
+    <t>LisConDepXlsDet</t>
+  </si>
+  <si>
+    <t>LisConDepXls</t>
+  </si>
+  <si>
+    <t>LisDepMesXlsDet</t>
+  </si>
+  <si>
+    <t>LisDepMesXlsRes</t>
+  </si>
+  <si>
+    <t>LISTEREJE</t>
+  </si>
+  <si>
+    <t>LisTraslPer</t>
+  </si>
+  <si>
+    <t>LisTrasl</t>
+  </si>
+  <si>
+    <t>logger_asserts</t>
+  </si>
+  <si>
+    <t>NumerosErroresActivosFijos</t>
+  </si>
+  <si>
+    <t>Persempr</t>
+  </si>
+  <si>
+    <t>PolManAct111</t>
+  </si>
+  <si>
+    <t>POLMANACT</t>
+  </si>
+  <si>
+    <t>PolManAct</t>
+  </si>
+  <si>
+    <t>PolSegAct</t>
+  </si>
+  <si>
+    <t>reportes_acfi</t>
+  </si>
+  <si>
+    <t>SinPolMan</t>
+  </si>
+  <si>
+    <t>subActAdi2</t>
+  </si>
+  <si>
+    <t>subActAdi</t>
+  </si>
+  <si>
+    <t>subActBaj</t>
+  </si>
+  <si>
+    <t>subActDes</t>
+  </si>
+  <si>
+    <t>subActImg</t>
+  </si>
+  <si>
+    <t>subActPer</t>
+  </si>
+  <si>
+    <t>subActTras</t>
+  </si>
+  <si>
+    <t>TrasActPer</t>
   </si>
 </sst>
 </file>
@@ -406,13 +505,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="52.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -423,21 +525,283 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>